<commit_message>
Setup: Added database documentation, modified homepage html to have a header, and misc test stuff
</commit_message>
<xml_diff>
--- a/Nutrient_Database_Tables.xlsx
+++ b/Nutrient_Database_Tables.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddaf326884c37f6a/Documents/Nutrient Tracker/Nutrient-Tracker/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_946C2C746BE8D0A762B6D915C56CB0E171A45FF8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759101B5-6323-4115-A404-8FC06D511C74}"/>
+  <bookViews>
+    <workbookView minimized="1" xWindow="2070" yWindow="3450" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Table 1</t>
   </si>
@@ -188,32 +197,41 @@
   </si>
   <si>
     <t>serving_size_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">going to have like mg is unit of measure. Basically storing the help text. Extend it for conversion. _ grams = _ ounces. 1 gram = 100 milligrams. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversions on a base 10. Like ounces in a gram. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -224,7 +242,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -246,54 +264,53 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -483,23 +500,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="10" width="18.88"/>
+    <col min="2" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,342 +529,359 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="F3" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="4" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="8" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="8" t="s">
+      <c r="F13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="8" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="8" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="8" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="8" t="s">
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -850,6 +889,6 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="B11:J11"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>